<commit_message>
Addressed case where metadata is indicated in a non-Stylus file. Also added wrapper function.
</commit_message>
<xml_diff>
--- a/in.xlsx
+++ b/in.xlsx
@@ -1,25 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfeoktistov\.spyder-py3\PortfolioUpdate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfeoktistov\Desktop\wo\Portfolio Update Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9135"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+  <si>
+    <t>Beep</t>
+  </si>
+  <si>
+    <t>Boop</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
   <si>
     <t>Label</t>
   </si>
@@ -27,24 +36,24 @@
     <t>DBID</t>
   </si>
   <si>
+    <t>F00000T770</t>
+  </si>
+  <si>
+    <t>1290 High Yield Bond A</t>
+  </si>
+  <si>
+    <t>Mfi</t>
+  </si>
+  <si>
+    <t>R1000.ind</t>
+  </si>
+  <si>
     <t>Russell 1000</t>
   </si>
   <si>
     <t>DEQ</t>
   </si>
   <si>
-    <t>Mfi</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>F00000T770</t>
-  </si>
-  <si>
-    <t>1290 High Yield Bond A</t>
-  </si>
-  <si>
     <t>F00000T772</t>
   </si>
   <si>
@@ -69,13 +78,20 @@
     <t>1290 Low Volatility Global Equity I</t>
   </si>
   <si>
-    <t>R1000.ind</t>
+    <t>MPI_Two</t>
+  </si>
+  <si>
+    <t>MPI_One</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -128,13 +144,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:QS50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,119 +476,149 @@
     <col min="9" max="9" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>5</v>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2">
-        <v>38657</v>
-      </c>
-      <c r="E1" s="2">
-        <v>43040</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>6.5566433665858197</v>
-      </c>
-      <c r="E2">
-        <v>6.5566433665858197</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
+        <v>38657</v>
+      </c>
+      <c r="E3" s="2">
+        <v>43040</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>6.5566433665858197</v>
+      </c>
+      <c r="E4">
+        <v>6.5566433665858197</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
         <v>5.782189526082357</v>
       </c>
-      <c r="E3">
+      <c r="E5">
         <v>5.782189526082357</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>4.5515376445559763</v>
+      </c>
+      <c r="E6">
+        <v>4.5515376445559763</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>1.2084169974967971</v>
+      </c>
+      <c r="E7">
+        <v>1.2084169974967971</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>2.7600254669288762</v>
+      </c>
+      <c r="E8">
+        <v>2.7600254669288762</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>4.5515376445559763</v>
-      </c>
-      <c r="E4">
-        <v>4.5515376445559763</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>1.2084169974967971</v>
-      </c>
-      <c r="E5">
-        <v>1.2084169974967971</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6">
-        <v>2.7600254669288762</v>
-      </c>
-      <c r="E6">
-        <v>2.7600254669288762</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7">
+      <c r="E9">
         <v>666</v>
       </c>
     </row>

</xml_diff>